<commit_message>
change to tiefaces 1.0.1 add validation page.
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
+++ b/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13080" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sale Price Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Configuration" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sale Price Report'!$A$1:$F$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sale Price Report'!$A$1:$F$8</definedName>
     <definedName name="solver_eng" localSheetId="0">1</definedName>
     <definedName name="solver_neg" localSheetId="0">1</definedName>
     <definedName name="solver_num" localSheetId="0">0</definedName>
-    <definedName name="solver_opt" localSheetId="0">'Sale Price Report'!$C$4</definedName>
+    <definedName name="solver_opt" localSheetId="0">'Sale Price Report'!$C$3</definedName>
     <definedName name="solver_typ" localSheetId="0">1</definedName>
     <definedName name="solver_val" localSheetId="0">0</definedName>
     <definedName name="solver_ver" localSheetId="0">3</definedName>
@@ -24,8 +23,75 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Jiang, Jason (MOHLTC)</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>tie:form(name="Sale Reports" length="7" headerLength="4" footerLength="0")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>tie:each(items="items", var="item", length="1" allowAdd="True")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>$validate{rule="$value&gt;0" error="Value must be greater than zero (0)."}
+$validate{rule="$value&lt;=500000" error="Value must be less than or equal to 500,000."}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>$validate{rule="$value&gt;0" error="Value must be greater than zero (0)."}</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sale Price Report</t>
   </si>
@@ -43,10 +109,6 @@
   </si>
   <si>
     <t>Sales</t>
-  </si>
-  <si>
-    <t>Price
-(&gt;0 and &lt;500000)</t>
   </si>
   <si>
     <t>Quantity
@@ -62,111 +124,20 @@
     <t>Note</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">  If you require help, please email to: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="10"/>
-        <color indexed="48"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Jason.Jiang.ca@gmail.com</t>
-    </r>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Tab Name</t>
-  </si>
-  <si>
-    <t>Sheet Name</t>
-  </si>
-  <si>
-    <t>Form Header Range</t>
-  </si>
-  <si>
-    <t>Form Body Range</t>
-  </si>
-  <si>
-    <t>Form Footer Range</t>
-  </si>
-  <si>
-    <t>Form Body Type</t>
-  </si>
-  <si>
-    <t>Allow ADD/DELETE ROW</t>
-  </si>
-  <si>
-    <t>Initial Rows</t>
-  </si>
-  <si>
-    <t>Form Page Type</t>
-  </si>
-  <si>
-    <t>Form Width</t>
-  </si>
-  <si>
-    <t>Max Rows Per Page</t>
-  </si>
-  <si>
-    <t>Saved Rows Before Repeat</t>
-  </si>
-  <si>
-    <t>Saved Rows After Repeat</t>
-  </si>
-  <si>
-    <t>Target Column/Cell</t>
-  </si>
-  <si>
-    <t>Attributes Type</t>
-  </si>
-  <si>
-    <t>Attributes Value</t>
-  </si>
-  <si>
-    <t>Validation Error Messages</t>
-  </si>
-  <si>
-    <t>$A$3 : $F$5</t>
-  </si>
-  <si>
-    <t>$A$6 : $F$9</t>
-  </si>
-  <si>
-    <t>Repeat</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
-    <t>$D</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>$value &gt;0 and $value &lt; 500000</t>
-  </si>
-  <si>
-    <t>Value must be greater than zero (0) and less than or equal to 500,000.</t>
-  </si>
-  <si>
-    <t>$E</t>
-  </si>
-  <si>
-    <t>$value &gt;0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value must be greater than zero (0) </t>
+    <t>${item.code}</t>
+  </si>
+  <si>
+    <t>${item.name}</t>
+  </si>
+  <si>
+    <t>${item.price}</t>
+  </si>
+  <si>
+    <t>${item.quantity}</t>
+  </si>
+  <si>
+    <t>Price
+(&gt;0 and &lt;=500000)</t>
   </si>
 </sst>
 </file>
@@ -174,9 +145,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -189,11 +160,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color indexed="8"/>
@@ -305,16 +271,17 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="48"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="25">
     <fill>
@@ -462,7 +429,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -662,149 +629,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="41" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="24" borderId="0" xfId="41" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="24" borderId="0" xfId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="4" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="21" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1149,296 +1101,142 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.5" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.33203125" style="2"/>
+    <col min="1" max="1" width="10.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="F1" s="9"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
     </row>
-    <row r="2" spans="1:6" ht="0.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="F2" s="9"/>
+    <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" ht="52.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <f>ROW()-4</f>
         <v>1</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="8" t="e">
+        <f>D5*E5</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
+    <row r="6" spans="1:6" s="2" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13" t="e">
+        <f>SUM((F5))</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="52.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="31"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>8</v>
-      </c>
+    <row r="7" spans="1:6" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
-    <row r="6" spans="1:6" s="8" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12">
-        <f>ROW()-5</f>
-        <v>1</v>
-      </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16">
-        <f>$D$6*$E$6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="8" customFormat="1" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20">
-        <f ca="1">SUM(INDIRECT("E6"):INDIRECT("E"&amp;TEXT(ROW()-1,"0")))</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
-        <f ca="1">SUM(INDIRECT("F6"):INDIRECT("F"&amp;TEXT(ROW()-1,"0")))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+    <row r="8" spans="1:6" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="8">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
+  <mergeCells count="7">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
   </mergeCells>
   <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.51111111111111107" footer="0.51111111111111107"/>
   <pageSetup scale="55" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q4"/>
-  <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="16.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="33.83203125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="9.33203125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" customWidth="1"/>
-    <col min="15" max="15" width="13.1640625" customWidth="1"/>
-    <col min="16" max="16" width="30.83203125" customWidth="1"/>
-    <col min="17" max="17" width="13.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="N4" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P4" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.51111111111111107" footer="0.51111111111111107"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
use adminFaces for bootstrap gui. Upgrade to tiefaces 1.0.4.
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
+++ b/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23892" windowHeight="10356" tabRatio="989"/>
+    <workbookView windowWidth="23895" windowHeight="10350" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sale Price Report" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,40 @@
     <definedName name="solver_val" localSheetId="0">0</definedName>
     <definedName name="solver_ver" localSheetId="0">3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>JASON</author>
     <author>Jiang, Jason (MOHLTC)</author>
   </authors>
   <commentList>
-    <comment ref="A5" authorId="0">
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">tie:form(name="Sale Price Report" length="7" headerLength="0" footerLength="0" fixedWidthStyle="true")
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -42,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0">
+    <comment ref="D5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -65,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="1">
       <text>
         <r>
           <rPr>
@@ -83,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>Sale Price Report</t>
   </si>
@@ -135,11 +158,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="5">
+    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="25">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -174,19 +201,158 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Times New Roman"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +377,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -314,10 +666,252 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -327,6 +921,27 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -345,7 +960,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -360,52 +975,73 @@
     <xf numFmtId="1" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 3" xfId="1"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Normal 2 3" xfId="49"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -690,132 +1326,132 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.33333333333333" defaultRowHeight="12.75" outlineLevelRow="7" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="10.4444444444444" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1111111111111" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.1111111111111" style="2" customWidth="1"/>
     <col min="4" max="4" width="23" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.33203125" style="2"/>
+    <col min="5" max="5" width="27.4444444444444" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.4444444444444" style="2" customWidth="1"/>
+    <col min="7" max="7" width="6.11111111111111" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.33333333333333" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1">
-      <c r="A1" s="16" t="s">
+    <row r="1" ht="33" customHeight="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="24" customHeight="1">
-      <c r="A2" s="17" t="s">
+    <row r="2" ht="24" customHeight="1" spans="1:6">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:6" ht="35.4" customHeight="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" ht="35.4" customHeight="1" spans="1:6">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="52.95" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="3" t="s">
+    <row r="4" ht="52.95" customHeight="1" spans="1:6">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="24.6" customHeight="1">
-      <c r="A5" s="4">
+    <row r="5" s="1" customFormat="1" ht="24.6" customHeight="1" spans="1:6">
+      <c r="A5" s="11">
         <f>ROW()-4</f>
         <v>1</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="8" t="e">
+      <c r="F5" s="15" t="e">
         <f>D5*E5</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="24.6" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" s="1" customFormat="1" ht="24.6" customHeight="1" spans="1:6">
+      <c r="A6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13" t="e">
+      <c r="B6" s="11"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="20" t="e">
         <f>SUM((F5))</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.95" customHeight="1">
-      <c r="A7" s="14" t="s">
+    <row r="7" ht="28.95" customHeight="1" spans="1:6">
+      <c r="A7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="21.6" customHeight="1">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+    <row r="8" ht="21.6" customHeight="1" spans="1:6">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -828,9 +1464,9 @@
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
   </mergeCells>
-  <pageMargins left="0.69791666666666696" right="0.69791666666666696" top="0.75" bottom="0.75" header="0.51041666666666696" footer="0.51041666666666696"/>
-  <pageSetup scale="55" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.697916666666667" right="0.697916666666667" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
+  <pageSetup paperSize="1" scale="55" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change charts to fixed layout
</commit_message>
<xml_diff>
--- a/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
+++ b/src/main/resources/websheet/PRICELISTINPUTVALIDATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350" tabRatio="989"/>
+    <workbookView windowWidth="19500" windowHeight="10350" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Sale Price Report" sheetId="1" r:id="rId1"/>
@@ -26,33 +26,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>JASON</author>
     <author>Jiang, Jason (MOHLTC)</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t xml:space="preserve">tie:form(name="Sale Price Report" length="7" headerLength="0" footerLength="0" fixedWidthStyle="true")
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <rFont val="Times New Roman"/>
-            <charset val="0"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A5" authorId="1">
+    <comment ref="A5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="1">
+    <comment ref="D5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -88,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="1">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -201,26 +178,39 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -240,43 +230,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -284,8 +237,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -293,30 +247,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,6 +261,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -338,6 +307,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -346,7 +323,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -379,19 +356,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,163 +536,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,6 +641,30 @@
         <color indexed="8"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -678,11 +679,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -702,21 +709,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -741,21 +733,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -767,148 +744,148 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1335,7 +1312,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="A1" sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.33333333333333" defaultRowHeight="12.75" outlineLevelRow="7" outlineLevelCol="5"/>

</xml_diff>